<commit_message>
create email verification, draft page, checkbox for publish
</commit_message>
<xml_diff>
--- a/public/EmployeeData/employee.xlsx
+++ b/public/EmployeeData/employee.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="49">
   <si>
     <t>No</t>
   </si>
@@ -64,7 +64,7 @@
     <t>Hidayat</t>
   </si>
   <si>
-    <t>rahmat@gmail.com</t>
+    <t>rahmattrust@gmail.com</t>
   </si>
   <si>
     <t>089912313213</t>
@@ -91,9 +91,6 @@
     <t>Juantoro</t>
   </si>
   <si>
-    <t>juan@gmail.com</t>
-  </si>
-  <si>
     <t>08212232133</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
   </si>
   <si>
     <t>FIkri</t>
-  </si>
-  <si>
-    <t>fikri@gmail.com</t>
   </si>
   <si>
     <t>08999654646</t>
@@ -175,8 +169,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="22">
@@ -202,83 +196,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -293,7 +226,84 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -308,38 +318,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -366,13 +360,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -384,163 +528,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -597,6 +591,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -608,21 +611,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -646,24 +634,32 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -686,163 +682,161 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -859,13 +853,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="48" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="48" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" quotePrefix="1"/>
   </cellXfs>
@@ -1219,7 +1206,7 @@
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelRow="7"/>
@@ -1227,7 +1214,7 @@
     <col min="1" max="1" width="5.66666666666667" customWidth="1"/>
     <col min="3" max="3" width="13.6666666666667" customWidth="1"/>
     <col min="4" max="4" width="16.5555555555556" customWidth="1"/>
-    <col min="5" max="5" width="13.5555555555556" customWidth="1"/>
+    <col min="5" max="5" width="23.8592592592593" customWidth="1"/>
     <col min="7" max="7" width="14.1333333333333" customWidth="1"/>
     <col min="8" max="8" width="15.7777777777778" customWidth="1"/>
     <col min="9" max="10" width="13" customWidth="1"/>
@@ -1294,31 +1281,31 @@
       <c r="E2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="8" t="s">
         <v>17</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="12">
+      <c r="K2" s="3">
         <v>5000000</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="L2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="M2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="12">
+      <c r="N2" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1335,34 +1322,34 @@
       <c r="D3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>26</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="12">
+      <c r="K3" s="3">
         <v>7400000</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="M3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="N3" s="12">
+      <c r="N3" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1374,39 +1361,39 @@
         <v>1124</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>30</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>32</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="I4" s="8" t="s">
+      <c r="H4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="12">
+      <c r="K4" s="3">
         <v>5300000</v>
       </c>
-      <c r="L4" s="12" t="s">
+      <c r="L4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="M4" s="12" t="s">
+      <c r="M4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="N4" s="12">
+      <c r="N4" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1418,39 +1405,39 @@
         <v>1125</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="F5" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>37</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="3">
         <v>5800000</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="L5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="M5" s="12" t="s">
+      <c r="M5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="N5" s="12">
+      <c r="N5" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1462,39 +1449,39 @@
         <v>1126</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="F6" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>41</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="J6" s="12" t="s">
+      <c r="I6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K6" s="12">
+      <c r="K6" s="3">
         <v>8200000</v>
       </c>
-      <c r="L6" s="12" t="s">
+      <c r="L6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="M6" s="12" t="s">
+      <c r="M6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="N6" s="12">
+      <c r="N6" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1506,39 +1493,39 @@
         <v>1127</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="F7" s="8" t="s">
         <v>44</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>46</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="J7" s="12" t="s">
+      <c r="H7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K7" s="12">
+      <c r="K7" s="3">
         <v>8400000</v>
       </c>
-      <c r="L7" s="12" t="s">
+      <c r="L7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="M7" s="12" t="s">
+      <c r="M7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="N7" s="12">
+      <c r="N7" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1550,51 +1537,51 @@
         <v>1128</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="F8" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>50</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J8" s="12" t="s">
+      <c r="J8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K8" s="12">
+      <c r="K8" s="3">
         <v>6800000</v>
       </c>
-      <c r="L8" s="12" t="s">
+      <c r="L8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="M8" s="12" t="s">
+      <c r="M8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="N8" s="12">
+      <c r="N8" s="3">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="rahmat@gmail.com" tooltip="mailto:rahmat@gmail.com"/>
-    <hyperlink ref="E3" r:id="rId2" display="juan@gmail.com"/>
-    <hyperlink ref="E4" r:id="rId3" display="fikri@gmail.com"/>
-    <hyperlink ref="E5" r:id="rId4" display="dareza@gmail.com"/>
-    <hyperlink ref="E6" r:id="rId5" display="agus@gmail.com" tooltip="mailto:agus@gmail.com"/>
-    <hyperlink ref="E7" r:id="rId6" display="ari@gmail.com" tooltip="mailto:ari@gmail.com"/>
-    <hyperlink ref="E8" r:id="rId7" display="aden@gmail.com" tooltip="mailto:aden@gmail.com"/>
+    <hyperlink ref="E2" r:id="rId1" display="rahmattrust@gmail.com" tooltip="mailto:rahmattrust@gmail.com"/>
+    <hyperlink ref="E3" r:id="rId1" display="rahmattrust@gmail.com" tooltip="mailto:rahmattrust@gmail.com"/>
+    <hyperlink ref="E4" r:id="rId1" display="rahmattrust@gmail.com" tooltip="mailto:rahmattrust@gmail.com"/>
+    <hyperlink ref="E5" r:id="rId2" display="dareza@gmail.com"/>
+    <hyperlink ref="E6" r:id="rId3" display="agus@gmail.com" tooltip="mailto:agus@gmail.com"/>
+    <hyperlink ref="E7" r:id="rId4" display="ari@gmail.com" tooltip="mailto:ari@gmail.com"/>
+    <hyperlink ref="E8" r:id="rId5" display="aden@gmail.com" tooltip="mailto:aden@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>

</xml_diff>